<commit_message>
log binning done; threading support for shortest distance
</commit_message>
<xml_diff>
--- a/graph/results/cz4071_summary.xlsx
+++ b/graph/results/cz4071_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edocsss/AEC/programming/CZ4071/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edocsss/AEC/programming/CZ4071/graph/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Degree Distribution</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Second Moment</t>
+  </si>
+  <si>
+    <t>Degree Exponent</t>
   </si>
 </sst>
 </file>
@@ -186,6 +189,94 @@
         <a:xfrm>
           <a:off x="7531100" y="101600"/>
           <a:ext cx="5998650" cy="4384800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>34600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>4413800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13817600" y="25400"/>
+          <a:ext cx="5851200" cy="4388400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>715600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>4562600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20281900" y="177800"/>
+          <a:ext cx="5846400" cy="4384800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -460,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:AE8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,7 +565,7 @@
     <col min="13" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="383" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" ht="383" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,8 +584,23 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -502,7 +608,7 @@
         <v>5.2650459515900199</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -510,9 +616,20 @@
         <v>2603.7240331662101</v>
       </c>
     </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.3298608219000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="B1:AE1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
A lot of things again
</commit_message>
<xml_diff>
--- a/graph/results/cz4071_summary.xlsx
+++ b/graph/results/cz4071_summary.xlsx
@@ -96,11 +96,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -120,94 +120,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>4498821</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1473200" y="114300"/>
-          <a:ext cx="5803900" cy="4384521"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>499550</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>4486400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7531100" y="101600"/>
-          <a:ext cx="5998650" cy="4384800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>787400</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -227,7 +139,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -271,7 +183,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -286,6 +198,94 @@
         <a:xfrm>
           <a:off x="20281900" y="177800"/>
           <a:ext cx="5846400" cy="4384800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>632460</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>4389120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7810500" y="0"/>
+          <a:ext cx="5852160" cy="4389120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>645160</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>4389120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866900" y="0"/>
+          <a:ext cx="5852160" cy="4389120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -563,7 +563,7 @@
   <dimension ref="A1:AE10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,36 +578,36 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -650,7 +650,7 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>5000</v>
       </c>
       <c r="B8" s="2">

</xml_diff>

<commit_message>
visualizations and other results
</commit_message>
<xml_diff>
--- a/graph/results/cz4071_summary.xlsx
+++ b/graph/results/cz4071_summary.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Degree Distribution</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>Clustering Coefficient Distribution</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Expected Degree Exponent</t>
   </si>
 </sst>
 </file>
@@ -116,12 +125,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -138,7 +153,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -154,6 +169,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -340,6 +358,50 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1866900" y="0"/>
+          <a:ext cx="5852160" cy="4389120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>670560</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>147320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7391400" y="5499100"/>
           <a:ext cx="5852160" cy="4389120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -615,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE23"/>
+  <dimension ref="A1:AE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,11 +757,33 @@
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B5" s="2">
+        <v>28754</v>
+      </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1134890</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2987624</v>
+      </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -740,46 +824,74 @@
       <c r="B15" s="2">
         <v>3545</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="2">
         <v>5.2793361262899996</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="2">
+        <v>8.0802277761899993E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="2">
+        <v>6.2185598180299999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2.3298608219000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2.3580093123100001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>